<commit_message>
u new img sizes
</commit_message>
<xml_diff>
--- a/0_dev/06b-new-img-sizes.xlsx
+++ b/0_dev/06b-new-img-sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/0_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBB1213-20B4-3F47-8CF4-BEAEFBA590F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64773C7F-E25D-CD49-BF29-7E1B5403FB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15540" activeTab="3" xr2:uid="{BDA854A8-7992-8C46-9CFC-4A708837B61C}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="25020" windowHeight="15540" activeTab="2" xr2:uid="{BDA854A8-7992-8C46-9CFC-4A708837B61C}"/>
   </bookViews>
   <sheets>
     <sheet name="100%" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D76A9C-D37C-2145-AF28-B49E3159F351}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D37B86C-A66C-2443-A26D-34CC86187F3C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1219,13 +1219,13 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>314</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
         <v>318</v>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3853A4-E9C5-2740-BB26-00D7402AC0D0}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G131" sqref="G12:G131"/>
     </sheetView>
   </sheetViews>

</xml_diff>